<commit_message>
Made some excersises. changed some things in DOE.py
</commit_message>
<xml_diff>
--- a/DOE/example.xlsx
+++ b/DOE/example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lteeg\Documents\Github\School\DOE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09615120-33A8-450E-BFF8-51E2AE7049F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25C7BC6C-C970-4A66-AE20-CC70827545ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5FEE7EB6-02AF-4463-922D-74F1A82BBF43}"/>
+    <workbookView xWindow="1884" yWindow="1884" windowWidth="17280" windowHeight="8880" xr2:uid="{5FEE7EB6-02AF-4463-922D-74F1A82BBF43}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
   <si>
     <t>treatment</t>
   </si>
@@ -60,57 +60,6 @@
   </si>
   <si>
     <t>fabric sample</t>
-  </si>
-  <si>
-    <t>1.3</t>
-  </si>
-  <si>
-    <t>1.6</t>
-  </si>
-  <si>
-    <t>0.5</t>
-  </si>
-  <si>
-    <t>1.2</t>
-  </si>
-  <si>
-    <t>1.1</t>
-  </si>
-  <si>
-    <t>2.2</t>
-  </si>
-  <si>
-    <t>2.4</t>
-  </si>
-  <si>
-    <t>0.4</t>
-  </si>
-  <si>
-    <t>2.0</t>
-  </si>
-  <si>
-    <t>1.8</t>
-  </si>
-  <si>
-    <t>1.7</t>
-  </si>
-  <si>
-    <t>0.6</t>
-  </si>
-  <si>
-    <t>1.5</t>
-  </si>
-  <si>
-    <t>3.9</t>
-  </si>
-  <si>
-    <t>4.4</t>
-  </si>
-  <si>
-    <t>4.1</t>
-  </si>
-  <si>
-    <t>3.4</t>
   </si>
 </sst>
 </file>
@@ -168,9 +117,6 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -178,6 +124,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -526,10 +475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F09A06BC-A649-4883-81B6-54303AEDBB20}">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -538,124 +487,116 @@
     <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="K3">
-        <f>_xlfn.F.DIST(75.13,4,5,FALSE)</f>
-        <v>3.8608953591679331E-6</v>
-      </c>
-      <c r="L3">
-        <f>_xlfn.F.DIST.RT(75.13,5,4)</f>
-        <v>4.8055197774933296E-4</v>
+      <c r="B3" s="4">
+        <v>1.3</v>
+      </c>
+      <c r="C3" s="4">
+        <v>1.6</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="E3" s="4">
+        <v>1.2</v>
+      </c>
+      <c r="F3" s="4">
+        <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>17</v>
+      <c r="B4" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C4" s="4">
+        <v>2.4</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="E4" s="4">
+        <v>2</v>
+      </c>
+      <c r="F4" s="4">
+        <v>1.8</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>8</v>
+      <c r="B5" s="4">
+        <v>1.8</v>
+      </c>
+      <c r="C5" s="4">
+        <v>1.7</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="E5" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="F5" s="4">
+        <v>1.3</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>24</v>
+      <c r="B6" s="4">
+        <v>3.9</v>
+      </c>
+      <c r="C6" s="4">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="D6" s="4">
+        <v>2</v>
+      </c>
+      <c r="E6" s="4">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="F6" s="4">
+        <v>3.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>